<commit_message>
Test case for DOSE_INFO files is working and passing
</commit_message>
<xml_diff>
--- a/tests/fixtures/dose_info_scanned.xlsx
+++ b/tests/fixtures/dose_info_scanned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4868D38B-15F9-6B49-96D1-6378379756BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1675A0E3-AA80-4D42-B441-9F536832E7E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6320" yWindow="3640" windowWidth="29340" windowHeight="15200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9060" yWindow="6600" windowWidth="29340" windowHeight="15200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>Configuration</t>
   </si>
@@ -114,9 +114,6 @@
     <t>10001</t>
   </si>
   <si>
-    <t>20200312</t>
-  </si>
-  <si>
     <t>Scan</t>
   </si>
   <si>
@@ -138,15 +135,9 @@
     <t>image-00001</t>
   </si>
   <si>
-    <t>img-with-pdf.dcm</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
-    <t>DICOM is an encapsulated report</t>
-  </si>
-  <si>
     <t>DICOM:Manufacturer</t>
   </si>
   <si>
@@ -175,6 +166,15 @@
   </si>
   <si>
     <t>tests/fixtures/dose_info/billybob-10001/20161223/Scan/dose_info.dcm</t>
+  </si>
+  <si>
+    <t>20161223</t>
+  </si>
+  <si>
+    <t>dose_info.dcm</t>
+  </si>
+  <si>
+    <t>DICOM has ImageType DOSE_INFO</t>
   </si>
 </sst>
 </file>
@@ -227,10 +227,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -643,7 +644,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -681,25 +682,25 @@
         <v>24</v>
       </c>
       <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" t="s">
         <v>41</v>
-      </c>
-      <c r="K1" t="s">
-        <v>42</v>
-      </c>
-      <c r="L1" t="s">
-        <v>43</v>
-      </c>
-      <c r="M1" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" t="s">
-        <v>44</v>
       </c>
       <c r="O1" t="s">
         <v>11</v>
       </c>
       <c r="P1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="Q1" t="s">
         <v>25</v>
@@ -719,7 +720,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -730,38 +731,38 @@
       <c r="F2" t="s">
         <v>29</v>
       </c>
-      <c r="G2">
-        <v>20161223</v>
+      <c r="G2" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" t="s">
         <v>31</v>
-      </c>
-      <c r="I2" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" t="s">
-        <v>32</v>
       </c>
       <c r="M2">
         <v>6168</v>
       </c>
-      <c r="O2" t="s">
-        <v>30</v>
+      <c r="O2" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="P2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" t="s">
         <v>33</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>34</v>
       </c>
       <c r="R2" t="s">
         <v>29</v>
       </c>
       <c r="S2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -769,10 +770,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
         <v>28</v>
@@ -780,52 +781,52 @@
       <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="G3">
-        <v>20161223</v>
+      <c r="G3" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" t="s">
         <v>31</v>
-      </c>
-      <c r="I3" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" t="s">
-        <v>32</v>
       </c>
       <c r="M3">
         <v>6168</v>
       </c>
-      <c r="O3" t="s">
-        <v>30</v>
+      <c r="O3" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="P3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" t="s">
         <v>33</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>34</v>
       </c>
       <c r="R3" t="s">
         <v>29</v>
       </c>
       <c r="S3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
         <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated expected dose-info test
</commit_message>
<xml_diff>
--- a/tests/fixtures/dose_info_scanned.xlsx
+++ b/tests/fixtures/dose_info_scanned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1675A0E3-AA80-4D42-B441-9F536832E7E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2513EC5B-DC67-CB49-B996-4F735C52B9FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9060" yWindow="6600" windowWidth="29340" windowHeight="15200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4700" yWindow="11300" windowWidth="29340" windowHeight="15200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="57">
   <si>
     <t>Configuration</t>
   </si>
@@ -175,6 +175,24 @@
   </si>
   <si>
     <t>DICOM has ImageType DOSE_INFO</t>
+  </si>
+  <si>
+    <t>tests/fixtures/dose_info/billybob-10001/20161223/Scan/image-00002.dcm</t>
+  </si>
+  <si>
+    <t>image-00002.dcm</t>
+  </si>
+  <si>
+    <t>image-00002</t>
+  </si>
+  <si>
+    <t>tests/fixtures/dose_info/billybob-10001/20161223/Scan/image-00003.dcm</t>
+  </si>
+  <si>
+    <t>image-00003.dcm</t>
+  </si>
+  <si>
+    <t>image-00003</t>
   </si>
 </sst>
 </file>
@@ -641,10 +659,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -816,16 +834,116 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
       <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4">
+        <v>6168</v>
+      </c>
+      <c r="O4" t="s">
+        <v>48</v>
+      </c>
+      <c r="P4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>33</v>
+      </c>
+      <c r="R4" t="s">
+        <v>29</v>
+      </c>
+      <c r="S4" t="s">
+        <v>30</v>
+      </c>
+      <c r="T4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M5">
+        <v>6168</v>
+      </c>
+      <c r="O5" t="s">
+        <v>48</v>
+      </c>
+      <c r="P5" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5" t="s">
+        <v>29</v>
+      </c>
+      <c r="S5" t="s">
+        <v>30</v>
+      </c>
+      <c r="T5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
         <v>47</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" t="s">
         <v>49</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D6" t="s">
         <v>37</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E6" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>